<commit_message>
Added in the final lab report pdf
</commit_message>
<xml_diff>
--- a/Lab2/data/Lab2.xlsx
+++ b/Lab2/data/Lab2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorti\Desktop\MSE 426\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorti\Desktop\MSE 426\MSE-426\Lab2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9411419-00AD-478D-938F-73BC6C82EAC3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40E82BB-C456-4E74-AFD4-16411EC3AA2B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="675" windowWidth="23535" windowHeight="15060" xr2:uid="{EE485BC8-4BBB-4153-85FF-E460F0E20EA9}"/>
+    <workbookView xWindow="60" yWindow="675" windowWidth="19170" windowHeight="15060" tabRatio="771" firstSheet="4" activeTab="8" xr2:uid="{EE485BC8-4BBB-4153-85FF-E460F0E20EA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Question 2-1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,10 @@
     <sheet name="Question 2-3" sheetId="3" r:id="rId3"/>
     <sheet name="Question 2-4" sheetId="4" r:id="rId4"/>
     <sheet name="Question 2-5" sheetId="5" r:id="rId5"/>
+    <sheet name="Question 3-1" sheetId="7" r:id="rId6"/>
+    <sheet name="Question 3-2" sheetId="8" r:id="rId7"/>
+    <sheet name="Question 3-3" sheetId="9" r:id="rId8"/>
+    <sheet name="Question 3-4" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="48">
   <si>
     <t>Question 2-1 Results</t>
   </si>
@@ -143,6 +147,42 @@
   </si>
   <si>
     <t>(5,5,5,5,5,5)</t>
+  </si>
+  <si>
+    <t>Question 3-1 Results</t>
+  </si>
+  <si>
+    <t>MaxFunctionEvaluations</t>
+  </si>
+  <si>
+    <t>fmincon (constrained): Optimality Tolerance</t>
+  </si>
+  <si>
+    <t>OptimalityTolerance</t>
+  </si>
+  <si>
+    <t>3000 (Default)</t>
+  </si>
+  <si>
+    <t>fmincon (constrained): MaxFunctionEvaluations</t>
+  </si>
+  <si>
+    <t>1e-6 (Default)</t>
+  </si>
+  <si>
+    <t>Question 3-3 Results</t>
+  </si>
+  <si>
+    <t>fmincon (constrained): Specify Objective Constrant: Set true (initially false as default)</t>
+  </si>
+  <si>
+    <t>fmincon (constrained): HessianApproximation (Use lbfgs instead of bfgs)</t>
+  </si>
+  <si>
+    <t>Question 3-4 Results</t>
+  </si>
+  <si>
+    <t>Question 3-2 Results</t>
   </si>
 </sst>
 </file>
@@ -212,11 +252,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -237,6 +274,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -555,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0782AAC4-1371-4161-8383-33E24F6E2510}">
   <dimension ref="B3:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,185 +610,185 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="B4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>1.0500000000000001E-2</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>0.29089999999999999</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>6.2023000000000001</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>3</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>15</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>0.94279999999999997</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>0.23899999999999999</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>7.6006</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>4</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>15</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>1.7955000000000001</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>0.15959999999999999</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>17.133199999999999</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>5</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <v>18</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>2.5754999999999999</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>0.06</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>40.361600000000003</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>6</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>21</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>0.52</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>0.2671</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>6.1608000000000001</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>49</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>201</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="3">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>3.2403</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>-4.5499999999999999E-2</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>80.159499999999994</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>14</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <v>66</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="3">
         <v>1</v>
       </c>
     </row>
@@ -775,231 +818,231 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="B4" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>0</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>0</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>0</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>0</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>0</v>
       </c>
-      <c r="H6" s="4">
-        <v>1</v>
-      </c>
-      <c r="I6" s="4">
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3">
         <v>45</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>2.6499999999999999E-2</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>-2.5999999999999999E-3</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>0.01</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>1.01E-2</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <v>9.9926000000000007E-7</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <v>25</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="3">
         <v>130</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>6.3E-3</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>-5.9999999999999995E-4</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>-1.24E-2</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>-1.24E-2</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <v>1.5612E-6</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="3">
         <v>26</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="3">
         <v>135</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>-2.4500000000000001E-2</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>2.3999999999999998E-3</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>-3.7000000000000002E-3</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <v>-3.7000000000000002E-3</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <v>1.8741E-6</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <v>32</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="5">
         <v>165</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>-3.0200000000000001E-2</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>-1.54E-2</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>-1.55E-2</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <v>1.7983E-6</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="3">
         <v>32</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="3">
         <v>170</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>3.3E-3</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>-2.9999999999999997E-4</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>-1.6299999999999999E-2</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>-1.6299999999999999E-2</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="4">
         <v>2.5702E-6</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="3">
         <v>37</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="3">
         <v>195</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1029,185 +1072,185 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>-5.6500000000000002E-2</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>2.0324</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>-4.5761000000000003</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>12</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>41</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>-5.6500000000000002E-2</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>2.0324</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>-4.5761000000000003</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>10</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>36</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>-5.6500000000000002E-2</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>2.0324</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>-4.5761000000000003</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>10</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <v>33</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>-5.6500000000000002E-2</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>2.0324</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>-4.5761000000000003</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>10</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>33</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>-5.6500000000000002E-2</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>2.0324</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>-4.5761000000000003</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>11</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>36</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>-5.6500000000000002E-2</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>2.0324</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>-4.5761000000000003</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>9</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <v>30</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1237,185 +1280,185 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>0.78639999999999999</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>0.61770000000000003</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>4.5699999999999998E-2</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>24</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>84</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>0.78639999999999999</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>0.61770000000000003</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>4.5699999999999998E-2</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>21</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>76</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>0.78639999999999999</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>0.61770000000000003</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>4.5699999999999998E-2</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>26</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <v>85</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>0.78639999999999999</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>0.61770000000000003</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>4.5699999999999998E-2</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>26</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>87</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>0.78639999999999999</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>0.61770000000000003</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>4.5699999999999998E-2</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>25</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>83</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>0.78639999999999999</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>0.61770000000000003</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>4.5699999999999998E-2</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>50</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <v>191</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1447,277 +1490,277 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>0</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>6</v>
       </c>
-      <c r="E6" s="4">
-        <v>1</v>
-      </c>
-      <c r="F6" s="4">
+      <c r="E6" s="3">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3">
         <v>0</v>
       </c>
-      <c r="G6" s="4">
-        <v>1</v>
-      </c>
-      <c r="H6" s="4">
+      <c r="G6" s="3">
+        <v>1</v>
+      </c>
+      <c r="H6" s="3">
         <v>0</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="3">
         <v>-147.99969999999999</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="3">
         <v>107</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="3">
         <v>107</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>0</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>6</v>
       </c>
-      <c r="E7" s="4">
-        <v>1</v>
-      </c>
-      <c r="F7" s="4">
+      <c r="E7" s="3">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3">
         <v>0</v>
       </c>
-      <c r="G7" s="4">
-        <v>1</v>
-      </c>
-      <c r="H7" s="4">
+      <c r="G7" s="3">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3">
         <v>0</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="3">
         <v>-147.99969999999999</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="3">
         <v>107</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="3">
         <v>107</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>5</v>
       </c>
-      <c r="D8" s="4">
-        <v>1</v>
-      </c>
-      <c r="E8" s="4">
-        <v>1</v>
-      </c>
-      <c r="F8" s="4">
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
         <v>0</v>
       </c>
-      <c r="G8" s="4">
-        <v>1</v>
-      </c>
-      <c r="H8" s="4">
+      <c r="G8" s="3">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3">
         <v>0</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="4">
         <v>-258</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="3">
         <v>12</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="3">
         <v>92</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>5</v>
       </c>
-      <c r="D9" s="6">
-        <v>1</v>
-      </c>
-      <c r="E9" s="6">
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5">
         <v>5</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <v>0</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="7">
         <v>5</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="8">
         <v>0</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="6">
         <v>-290</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="5">
         <v>77</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="5">
         <v>77</v>
       </c>
-      <c r="L9" s="6">
+      <c r="L9" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>5</v>
       </c>
-      <c r="D10" s="4">
-        <v>1</v>
-      </c>
-      <c r="E10" s="4">
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3">
         <v>5</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>0</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>5</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="3">
         <v>0</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="4">
         <v>-290</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="3">
         <v>98</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="3">
         <v>98</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>5</v>
       </c>
-      <c r="D11" s="4">
-        <v>1</v>
-      </c>
-      <c r="E11" s="4">
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3">
         <v>5</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>6</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <v>5</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="3">
         <v>10</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="4">
         <v>-298</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="3">
         <v>86</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="3">
         <v>86</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L11" s="3">
         <v>1</v>
       </c>
     </row>
@@ -1729,4 +1772,792 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BE41236-3602-4059-95F5-C943C57EDB78}">
+  <dimension ref="B3:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="3" max="6" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>3</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3">
+        <v>-9.11E-2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1.9745999999999999</v>
+      </c>
+      <c r="E7" s="3">
+        <v>-4.5324999999999998</v>
+      </c>
+      <c r="F7" s="3">
+        <v>3</v>
+      </c>
+      <c r="G7" s="3">
+        <v>12</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="3">
+        <v>-5.6500000000000002E-2</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2.0324</v>
+      </c>
+      <c r="E8" s="3">
+        <v>-4.5761000000000003</v>
+      </c>
+      <c r="F8" s="3">
+        <v>10</v>
+      </c>
+      <c r="G8" s="3">
+        <v>33</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="10">
+        <v>1E-3</v>
+      </c>
+      <c r="C9" s="3">
+        <v>-5.6500000000000002E-2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2.0316000000000001</v>
+      </c>
+      <c r="E9" s="3">
+        <v>-4.5753000000000004</v>
+      </c>
+      <c r="F9" s="3">
+        <v>7</v>
+      </c>
+      <c r="G9" s="3">
+        <v>24</v>
+      </c>
+      <c r="H9" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="10">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="C10" s="3">
+        <v>-5.6500000000000002E-2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2.0324</v>
+      </c>
+      <c r="E10" s="3">
+        <v>-4.5761000000000003</v>
+      </c>
+      <c r="F10" s="3">
+        <v>12</v>
+      </c>
+      <c r="G10" s="3">
+        <v>48</v>
+      </c>
+      <c r="H10" s="3">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7DA056C-5C18-45CB-826A-976DFA4523C7}">
+  <dimension ref="B3:H10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="3" max="6" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="3">
+        <v>-5.6500000000000002E-2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2.0324</v>
+      </c>
+      <c r="E6" s="3">
+        <v>-4.5761000000000003</v>
+      </c>
+      <c r="F6" s="3">
+        <v>10</v>
+      </c>
+      <c r="G6" s="3">
+        <v>36</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <v>100</v>
+      </c>
+      <c r="C7" s="3">
+        <v>-5.6500000000000002E-2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2.0324</v>
+      </c>
+      <c r="E7" s="3">
+        <v>-4.5761000000000003</v>
+      </c>
+      <c r="F7" s="3">
+        <v>10</v>
+      </c>
+      <c r="G7" s="3">
+        <v>33</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>50</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1.7955000000000001</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.15959999999999999</v>
+      </c>
+      <c r="E8" s="3">
+        <v>17.133199999999999</v>
+      </c>
+      <c r="F8" s="3">
+        <v>5</v>
+      </c>
+      <c r="G8" s="3">
+        <v>18</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
+        <v>30</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2.5754999999999999</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.06</v>
+      </c>
+      <c r="E9" s="3">
+        <v>40.361600000000003</v>
+      </c>
+      <c r="F9" s="3">
+        <v>6</v>
+      </c>
+      <c r="G9" s="3">
+        <v>21</v>
+      </c>
+      <c r="H9" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="2">
+        <v>20</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.52</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.2671</v>
+      </c>
+      <c r="E10" s="3">
+        <v>6.1608000000000001</v>
+      </c>
+      <c r="F10" s="3">
+        <v>49</v>
+      </c>
+      <c r="G10" s="3">
+        <v>201</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7390A960-0F43-4368-AAC5-63A437D658A9}">
+  <dimension ref="B3:H11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="6" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="3">
+        <v>-5.6500000000000002E-2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2.0324</v>
+      </c>
+      <c r="E6" s="3">
+        <v>-4.5761000000000003</v>
+      </c>
+      <c r="F6" s="3">
+        <v>12</v>
+      </c>
+      <c r="G6" s="3">
+        <v>41</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3">
+        <v>-5.6500000000000002E-2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2.0324</v>
+      </c>
+      <c r="E7" s="3">
+        <v>-4.5761000000000003</v>
+      </c>
+      <c r="F7" s="3">
+        <v>10</v>
+      </c>
+      <c r="G7" s="3">
+        <v>36</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3">
+        <v>-5.6500000000000002E-2</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2.0324</v>
+      </c>
+      <c r="E8" s="3">
+        <v>-4.5761000000000003</v>
+      </c>
+      <c r="F8" s="3">
+        <v>10</v>
+      </c>
+      <c r="G8" s="3">
+        <v>33</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="3">
+        <v>-5.6500000000000002E-2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2.0324</v>
+      </c>
+      <c r="E9" s="3">
+        <v>-4.5761000000000003</v>
+      </c>
+      <c r="F9" s="3">
+        <v>10</v>
+      </c>
+      <c r="G9" s="3">
+        <v>33</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="3">
+        <v>-5.6500000000000002E-2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2.0324</v>
+      </c>
+      <c r="E10" s="3">
+        <v>-4.5761000000000003</v>
+      </c>
+      <c r="F10" s="3">
+        <v>11</v>
+      </c>
+      <c r="G10" s="3">
+        <v>36</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="3">
+        <v>-5.6500000000000002E-2</v>
+      </c>
+      <c r="D11" s="3">
+        <v>2.0324</v>
+      </c>
+      <c r="E11" s="3">
+        <v>-4.5761000000000003</v>
+      </c>
+      <c r="F11" s="3">
+        <v>9</v>
+      </c>
+      <c r="G11" s="3">
+        <v>30</v>
+      </c>
+      <c r="H11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF4D24C0-42E1-42E2-B97E-BD51D8E953DC}">
+  <dimension ref="B3:H11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="6" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="3">
+        <v>-5.6500000000000002E-2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2.0324</v>
+      </c>
+      <c r="E6" s="3">
+        <v>-4.5761000000000003</v>
+      </c>
+      <c r="F6" s="3">
+        <v>13</v>
+      </c>
+      <c r="G6" s="3">
+        <v>44</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3">
+        <v>-5.6500000000000002E-2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2.0324</v>
+      </c>
+      <c r="E7" s="3">
+        <v>-4.5761000000000003</v>
+      </c>
+      <c r="F7" s="3">
+        <v>13</v>
+      </c>
+      <c r="G7" s="3">
+        <v>46</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3">
+        <v>-5.6500000000000002E-2</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2.0324</v>
+      </c>
+      <c r="E8" s="3">
+        <v>-4.5761000000000003</v>
+      </c>
+      <c r="F8" s="3">
+        <v>11</v>
+      </c>
+      <c r="G8" s="3">
+        <v>36</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="3">
+        <v>-5.6500000000000002E-2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2.0324</v>
+      </c>
+      <c r="E9" s="3">
+        <v>-4.5761000000000003</v>
+      </c>
+      <c r="F9" s="3">
+        <v>12</v>
+      </c>
+      <c r="G9" s="3">
+        <v>39</v>
+      </c>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="3">
+        <v>-5.6500000000000002E-2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2.0324</v>
+      </c>
+      <c r="E10" s="3">
+        <v>-4.5761000000000003</v>
+      </c>
+      <c r="F10" s="3">
+        <v>13</v>
+      </c>
+      <c r="G10" s="3">
+        <v>42</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="3">
+        <v>-5.6500000000000002E-2</v>
+      </c>
+      <c r="D11" s="3">
+        <v>2.0324</v>
+      </c>
+      <c r="E11" s="3">
+        <v>-4.5761000000000003</v>
+      </c>
+      <c r="F11" s="3">
+        <v>12</v>
+      </c>
+      <c r="G11" s="3">
+        <v>39</v>
+      </c>
+      <c r="H11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>